<commit_message>
Added model # details, sru233 changes, sr-smart api
</commit_message>
<xml_diff>
--- a/General/SR Smart Model #.xlsx
+++ b/General/SR Smart Model #.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCiTeR\Github\SecuRemote\General\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ashok\SecuRemote\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5235" windowHeight="4050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760"/>
   </bookViews>
   <sheets>
     <sheet name="SR Samrt Product model #" sheetId="1" r:id="rId1"/>
     <sheet name="Legacy_product_model #" sheetId="3" r:id="rId2"/>
     <sheet name="Version_History" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="282">
   <si>
     <t>Designator communication trade name</t>
   </si>
@@ -389,9 +389,6 @@
     <t>SRD231</t>
   </si>
   <si>
-    <t>Develper Kit V4.0 Nordic BLE and ANT</t>
-  </si>
-  <si>
     <t>SRR232</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>2AEHJ</t>
   </si>
   <si>
-    <t>SRH232</t>
-  </si>
-  <si>
     <t>SR Host board for testing SRU232</t>
   </si>
   <si>
@@ -801,6 +795,78 @@
   </si>
   <si>
     <t>SR Smart Bridge Nordic BLE and ANT using Ethernet</t>
+  </si>
+  <si>
+    <t>SRW532</t>
+  </si>
+  <si>
+    <t>SR WMN Eval kit</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Wireless Mesh Network Test kit</t>
+  </si>
+  <si>
+    <t>SR COO for WMN Test Kit</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SR Module Test Device for WMN Test Kit</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR OEM PoC </t>
+  </si>
+  <si>
+    <t>SRO532</t>
+  </si>
+  <si>
+    <t>SRM532</t>
+  </si>
+  <si>
+    <t>SR COO for WMN Eval Kit</t>
+  </si>
+  <si>
+    <t>01.01.10</t>
+  </si>
+  <si>
+    <t>added SRW532, SRC532, SRM532, added category O for OEM</t>
+  </si>
+  <si>
+    <t>DEVSRH232</t>
+  </si>
+  <si>
+    <t>SR DevKit - 2 using SRU232 module</t>
+  </si>
+  <si>
+    <t>Develper Kit V3.0 Nordic BLE module SRD531</t>
+  </si>
+  <si>
+    <t>Old devkit, Obsolete</t>
+  </si>
+  <si>
+    <t>SRM533</t>
+  </si>
+  <si>
+    <t>SR Module Testing Device for WMN Eval Kit using Long Range Module, SRU232</t>
+  </si>
+  <si>
+    <t>SR Module Testing Device for WMN Eval Kit, using Short Range Module, SRU233</t>
+  </si>
+  <si>
+    <t>01.01.11</t>
+  </si>
+  <si>
+    <t>Added SRM233</t>
+  </si>
+  <si>
+    <t>DEVSRJ232</t>
   </si>
 </sst>
 </file>
@@ -1113,18 +1179,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1134,14 +1188,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1154,6 +1205,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1438,289 +1504,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:P84"/>
+  <dimension ref="A4:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68:L68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="36.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
+    <col min="13" max="13" width="36.08984375" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43" t="s">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="G4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="42"/>
+      <c r="I5" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="41"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="43"/>
       <c r="C6" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="I6" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="I6" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="42"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G7" s="36"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="I8" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="45"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="42"/>
+      <c r="F8" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="47"/>
+      <c r="I8" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="43"/>
       <c r="C9" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="51" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9" s="52"/>
-      <c r="I9" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="45"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="42"/>
+      <c r="F9" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="47"/>
+      <c r="I9" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="43"/>
       <c r="C10" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="50"/>
-      <c r="I10" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="F10" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="I10" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="14" t="s">
-        <v>147</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="I11" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="42"/>
+      <c r="F11" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="I11" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="43"/>
       <c r="C12" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="42"/>
+        <v>143</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="43"/>
       <c r="C13" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="I13" s="43" t="s">
-        <v>231</v>
-      </c>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="45"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="42"/>
+        <v>143</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="43"/>
       <c r="C14" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>230</v>
-      </c>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="42"/>
+        <v>213</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="43"/>
       <c r="C15" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I15" s="43" t="s">
-        <v>230</v>
-      </c>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="F16" s="6"/>
@@ -1730,7 +1797,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="18" spans="3:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1806,7 @@
       </c>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>2</v>
       </c>
@@ -1747,7 +1814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>3</v>
       </c>
@@ -1758,10 +1825,10 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>7</v>
       </c>
@@ -1775,7 +1842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H22" t="s">
         <v>11</v>
       </c>
@@ -1783,7 +1850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H23" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +1869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H25" t="s">
         <v>18</v>
       </c>
@@ -1810,7 +1877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H26" t="s">
         <v>20</v>
       </c>
@@ -1818,7 +1885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
         <v>22</v>
       </c>
@@ -1826,7 +1893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
         <v>24</v>
       </c>
@@ -1834,7 +1901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H29" t="s">
         <v>26</v>
       </c>
@@ -1842,7 +1909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H30" t="s">
         <v>28</v>
       </c>
@@ -1850,665 +1917,646 @@
         <v>29</v>
       </c>
       <c r="K30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H31" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
         <v>167</v>
       </c>
-      <c r="I31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+      <c r="I32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>198</v>
+      </c>
+      <c r="I34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>225</v>
+      </c>
+      <c r="I35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>260</v>
+      </c>
+      <c r="I36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>263</v>
+      </c>
+      <c r="I37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>265</v>
+      </c>
+      <c r="I38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>31</v>
+      </c>
+      <c r="K40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B43" s="20">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43">
+        <v>7</v>
+      </c>
+      <c r="L43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B44" s="20"/>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+      <c r="L44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="25">
+        <v>2</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="10">
+        <v>2</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K45" s="10">
+        <v>1</v>
+      </c>
+      <c r="L45" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="M45" s="50"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B46" s="20">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46" t="s">
+        <v>41</v>
+      </c>
+      <c r="K46">
+        <v>2</v>
+      </c>
+      <c r="L46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B47" s="20">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="L47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B48" s="20">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>234</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="L48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B49" s="20">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>161</v>
+      </c>
+      <c r="G49">
+        <v>6</v>
+      </c>
+      <c r="H49" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B50" s="20">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+      <c r="L50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B51" s="20">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>46</v>
+      </c>
+      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="L51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B52" s="20">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52">
+        <v>9</v>
+      </c>
+      <c r="H52" t="s">
+        <v>49</v>
+      </c>
+      <c r="K52">
+        <v>8</v>
+      </c>
+      <c r="L52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B53" s="8"/>
+      <c r="K53">
+        <v>9</v>
+      </c>
+      <c r="L53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B54" s="8"/>
+      <c r="K54" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="L54" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="M54" s="19"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B55" s="8"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="C59" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B60" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" t="s">
+        <v>52</v>
+      </c>
+      <c r="N60" t="s">
+        <v>123</v>
+      </c>
+      <c r="O60" t="s">
+        <v>124</v>
+      </c>
+      <c r="P60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B61" s="20">
+        <v>110</v>
+      </c>
+      <c r="C61" t="s">
+        <v>142</v>
+      </c>
+      <c r="E61" t="s">
+        <v>157</v>
+      </c>
+      <c r="M61" t="s">
+        <v>159</v>
+      </c>
+      <c r="N61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="25">
+        <v>137</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="M62" s="24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B63" s="20">
+        <v>137</v>
+      </c>
+      <c r="C63" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" t="s">
+        <v>158</v>
+      </c>
+      <c r="M63" t="s">
+        <v>159</v>
+      </c>
+      <c r="N63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B64" s="20">
+        <v>175</v>
+      </c>
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="52"/>
+      <c r="M64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B65" s="20">
+        <v>175</v>
+      </c>
+      <c r="C65" t="s">
+        <v>162</v>
+      </c>
+      <c r="E65" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B66" s="20">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
+        <v>108</v>
+      </c>
+      <c r="E66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B67" s="20">
+        <v>163</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="E67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="25">
         <v>169</v>
       </c>
-      <c r="I32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H33" t="s">
-        <v>173</v>
-      </c>
-      <c r="I33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H34" t="s">
-        <v>200</v>
-      </c>
-      <c r="I34" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
+      <c r="C68" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D68" s="30"/>
+      <c r="E68" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="42"/>
+      <c r="J68" s="42"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B69" s="20">
+        <v>171</v>
+      </c>
+      <c r="C69" t="s">
+        <v>114</v>
+      </c>
+      <c r="E69" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="25">
+        <v>179</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="N70" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="O70" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="I35" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>30</v>
-      </c>
-      <c r="G38" t="s">
-        <v>31</v>
-      </c>
-      <c r="K38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" t="s">
-        <v>34</v>
-      </c>
-      <c r="K39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="20">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>36</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" t="s">
-        <v>37</v>
-      </c>
-      <c r="K41">
-        <v>7</v>
-      </c>
-      <c r="L41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42" t="s">
-        <v>39</v>
-      </c>
-      <c r="K42">
-        <v>3</v>
-      </c>
-      <c r="L42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="25">
-        <v>2</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G43" s="10">
-        <v>2</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K43" s="10">
-        <v>1</v>
-      </c>
-      <c r="L43" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="M43" s="41"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="20">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>152</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="H44" t="s">
-        <v>41</v>
-      </c>
-      <c r="K44">
-        <v>2</v>
-      </c>
-      <c r="L44" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="20">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45">
-        <v>4</v>
-      </c>
-      <c r="H45" t="s">
-        <v>43</v>
-      </c>
-      <c r="K45">
-        <v>3</v>
-      </c>
-      <c r="L45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="20">
-        <v>5</v>
-      </c>
-      <c r="C46" t="s">
-        <v>236</v>
-      </c>
-      <c r="G46">
-        <v>5</v>
-      </c>
-      <c r="H46" t="s">
-        <v>44</v>
-      </c>
-      <c r="K46">
-        <v>4</v>
-      </c>
-      <c r="L46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="20">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>162</v>
-      </c>
-      <c r="G47">
-        <v>6</v>
-      </c>
-      <c r="H47" t="s">
-        <v>45</v>
-      </c>
-      <c r="K47">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="20">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B71" s="20">
+        <v>180</v>
+      </c>
+      <c r="C71" t="s">
         <v>153</v>
       </c>
-      <c r="G48">
-        <v>7</v>
-      </c>
-      <c r="H48" t="s">
-        <v>45</v>
-      </c>
-      <c r="K48">
-        <v>6</v>
-      </c>
-      <c r="L48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="20">
-        <v>8</v>
-      </c>
-      <c r="C49" t="s">
-        <v>46</v>
-      </c>
-      <c r="K49">
-        <v>7</v>
-      </c>
-      <c r="L49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="20">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G50">
-        <v>9</v>
-      </c>
-      <c r="H50" t="s">
-        <v>49</v>
-      </c>
-      <c r="K50">
-        <v>8</v>
-      </c>
-      <c r="L50" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
-      <c r="K51">
-        <v>9</v>
-      </c>
-      <c r="L51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
-      <c r="K52" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="L52" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="M52" s="19"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B58" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" t="s">
-        <v>52</v>
-      </c>
-      <c r="N58" t="s">
-        <v>124</v>
-      </c>
-      <c r="O58" t="s">
-        <v>125</v>
-      </c>
-      <c r="P58" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B59" s="20">
-        <v>110</v>
-      </c>
-      <c r="C59" t="s">
-        <v>143</v>
-      </c>
-      <c r="E59" t="s">
-        <v>158</v>
-      </c>
-      <c r="M59" t="s">
-        <v>160</v>
-      </c>
-      <c r="N59" t="s">
+      <c r="E71" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
+      <c r="L71" s="38"/>
+      <c r="M71" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B72" s="20">
+        <v>187</v>
+      </c>
+      <c r="C72" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
+      <c r="L72" s="52"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="25">
-        <v>137</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="M60" s="24" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B61" s="20">
-        <v>137</v>
-      </c>
-      <c r="C61" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" t="s">
-        <v>159</v>
-      </c>
-      <c r="M61" t="s">
-        <v>160</v>
-      </c>
-      <c r="N61" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B62" s="20">
-        <v>175</v>
-      </c>
-      <c r="C62" t="s">
-        <v>123</v>
-      </c>
-      <c r="E62" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="F62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-      <c r="J62" s="38"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="39"/>
-      <c r="M62" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B63" s="20">
-        <v>175</v>
-      </c>
-      <c r="C63" t="s">
-        <v>163</v>
-      </c>
-      <c r="E63" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="38"/>
-      <c r="K63" s="38"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B64" s="20">
-        <v>163</v>
-      </c>
-      <c r="C64" t="s">
-        <v>108</v>
-      </c>
-      <c r="E64" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" s="20">
-        <v>163</v>
-      </c>
-      <c r="C65" t="s">
-        <v>110</v>
-      </c>
-      <c r="E65" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="25">
-        <v>169</v>
-      </c>
-      <c r="C66" s="30" t="s">
-        <v>220</v>
-      </c>
-      <c r="D66" s="30"/>
-      <c r="E66" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="48"/>
-      <c r="K66" s="48"/>
-      <c r="L66" s="48"/>
-      <c r="M66" s="10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B67" s="20">
-        <v>171</v>
-      </c>
-      <c r="C67" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="25">
-        <v>179</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="N68" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="O68" s="26" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="20">
-        <v>180</v>
-      </c>
-      <c r="C69" t="s">
-        <v>154</v>
-      </c>
-      <c r="E69" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="19"/>
-      <c r="N69" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O69" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B70" s="20">
-        <v>187</v>
-      </c>
-      <c r="C70" t="s">
-        <v>119</v>
-      </c>
-      <c r="E70" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="F70" s="38"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="38"/>
-      <c r="L70" s="39"/>
-      <c r="M70" s="23"/>
-      <c r="N70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="P70" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B71" s="29">
-        <v>188</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="D71" s="19"/>
-      <c r="E71" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="F71" s="40"/>
-      <c r="G71" s="40"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="40"/>
-      <c r="J71" s="40"/>
-      <c r="K71" s="40"/>
-      <c r="L71" s="40"/>
-      <c r="M71" t="s">
-        <v>238</v>
-      </c>
-      <c r="N71" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O71" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B72" s="29">
-        <v>188</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="F72" s="40"/>
-      <c r="G72" s="40"/>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
-      <c r="J72" s="40"/>
-      <c r="K72" s="40"/>
-      <c r="L72" s="40"/>
-      <c r="M72" t="s">
-        <v>242</v>
-      </c>
-      <c r="N72" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="O72" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B73" s="29">
         <v>188</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="E73" s="40" t="s">
-        <v>256</v>
-      </c>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="40"/>
-      <c r="L73" s="40"/>
+        <v>237</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="F73" s="51"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="51"/>
+      <c r="J73" s="51"/>
+      <c r="K73" s="51"/>
+      <c r="L73" s="51"/>
       <c r="M73" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B74" s="20">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B74" s="29">
+        <v>188</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="F74" s="51"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="51"/>
+      <c r="K74" s="51"/>
+      <c r="L74" s="51"/>
+      <c r="M74" t="s">
+        <v>240</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="29">
+        <v>188</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="E75" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="F75" s="51"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="51"/>
+      <c r="J75" s="51"/>
+      <c r="K75" s="51"/>
+      <c r="L75" s="51"/>
+      <c r="M75" t="s">
+        <v>240</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B76" s="20">
         <v>191</v>
       </c>
-      <c r="C74" t="s">
-        <v>176</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="F74" s="38"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="L74" s="38"/>
-      <c r="M74" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B75" s="20">
-        <v>192</v>
-      </c>
-      <c r="C75" t="s">
-        <v>165</v>
-      </c>
-      <c r="E75" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
-      <c r="L75" s="38"/>
-      <c r="N75" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B76" s="20">
-        <v>193</v>
-      </c>
       <c r="C76" t="s">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="E76" s="38" t="s">
-        <v>171</v>
+        <v>251</v>
       </c>
       <c r="F76" s="38"/>
       <c r="G76" s="38"/>
@@ -2518,212 +2566,387 @@
       <c r="K76" s="38"/>
       <c r="L76" s="38"/>
       <c r="M76" t="s">
-        <v>245</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O76" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B77" s="20">
+        <v>192</v>
+      </c>
+      <c r="C77" t="s">
+        <v>272</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="38"/>
+      <c r="N77" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B78" s="20">
+        <v>193</v>
+      </c>
+      <c r="C78" t="s">
+        <v>267</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="38"/>
+      <c r="M78" t="s">
+        <v>243</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B79" s="20">
         <v>194</v>
       </c>
-      <c r="E77" s="40" t="s">
+      <c r="E79" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="51"/>
+      <c r="I79" s="51"/>
+      <c r="J79" s="51"/>
+      <c r="K79" s="51"/>
+      <c r="L79" s="51"/>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B80" s="29">
+        <v>195</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D80" s="19"/>
+      <c r="E80" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="F80" s="51"/>
+      <c r="G80" s="51"/>
+      <c r="H80" s="51"/>
+      <c r="I80" s="51"/>
+      <c r="J80" s="51"/>
+      <c r="K80" s="51"/>
+      <c r="L80" s="51"/>
+      <c r="M80" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="N80" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="O80" s="23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B81" s="29">
+        <v>196</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="19"/>
+      <c r="E81" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="40"/>
-      <c r="K77" s="40"/>
-      <c r="L77" s="40"/>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B78" s="29">
-        <v>195</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="40"/>
-      <c r="K78" s="40"/>
-      <c r="L78" s="40"/>
-      <c r="M78" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="N78" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="O78" s="23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B79" s="29">
-        <v>196</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="F79" s="40"/>
-      <c r="G79" s="40"/>
-      <c r="H79" s="40"/>
-      <c r="I79" s="40"/>
-      <c r="J79" s="40"/>
-      <c r="K79" s="40"/>
-      <c r="L79" s="40"/>
-      <c r="N79" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="O79" s="23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B80" s="20">
-        <v>157</v>
-      </c>
-      <c r="C80" t="s">
-        <v>222</v>
-      </c>
-      <c r="E80" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="40"/>
-      <c r="J80" s="40"/>
-      <c r="K80" s="40"/>
-      <c r="L80" s="40"/>
-      <c r="N80" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="20">
-        <v>157</v>
-      </c>
-      <c r="C81" t="s">
-        <v>224</v>
-      </c>
-      <c r="E81" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="F81" s="40"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="40"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="40"/>
-      <c r="K81" s="40"/>
-      <c r="L81" s="40"/>
-      <c r="N81" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="O81" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F81" s="51"/>
+      <c r="G81" s="51"/>
+      <c r="H81" s="51"/>
+      <c r="I81" s="51"/>
+      <c r="J81" s="51"/>
+      <c r="K81" s="51"/>
+      <c r="L81" s="51"/>
+      <c r="N81" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="O81" s="23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B82" s="20">
         <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>223</v>
-      </c>
-      <c r="E82" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="E82" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="F82" s="40"/>
-      <c r="G82" s="40"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="40"/>
-      <c r="J82" s="40"/>
-      <c r="K82" s="40"/>
-      <c r="L82" s="40"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="51"/>
+      <c r="I82" s="51"/>
+      <c r="J82" s="51"/>
+      <c r="K82" s="51"/>
+      <c r="L82" s="51"/>
       <c r="N82" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B83" s="20">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="C83" t="s">
-        <v>233</v>
-      </c>
-      <c r="E83" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="E83" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="F83" s="40"/>
-      <c r="G83" s="40"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40"/>
-      <c r="K83" s="40"/>
-      <c r="L83" s="40"/>
+      <c r="F83" s="51"/>
+      <c r="G83" s="51"/>
+      <c r="H83" s="51"/>
+      <c r="I83" s="51"/>
+      <c r="J83" s="51"/>
+      <c r="K83" s="51"/>
+      <c r="L83" s="51"/>
       <c r="N83" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B84" s="20">
         <v>157</v>
       </c>
       <c r="C84" t="s">
-        <v>235</v>
-      </c>
-      <c r="E84" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E84" s="51" t="s">
         <v>248</v>
       </c>
-      <c r="F84" s="38"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="38"/>
-      <c r="J84" s="38"/>
-      <c r="K84" s="38"/>
-      <c r="L84" s="38"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="51"/>
+      <c r="I84" s="51"/>
+      <c r="J84" s="51"/>
+      <c r="K84" s="51"/>
+      <c r="L84" s="51"/>
       <c r="N84" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B85" s="20">
+        <v>188</v>
+      </c>
+      <c r="C85" t="s">
+        <v>231</v>
+      </c>
+      <c r="E85" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="F85" s="51"/>
+      <c r="G85" s="51"/>
+      <c r="H85" s="51"/>
+      <c r="I85" s="51"/>
+      <c r="J85" s="51"/>
+      <c r="K85" s="51"/>
+      <c r="L85" s="51"/>
+      <c r="N85" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B86" s="20">
+        <v>157</v>
+      </c>
+      <c r="C86" t="s">
+        <v>233</v>
+      </c>
+      <c r="E86" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="F86" s="38"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="38"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="38"/>
+      <c r="L86" s="38"/>
+      <c r="N86" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B87" s="20">
+        <v>179</v>
+      </c>
+      <c r="C87" t="s">
+        <v>258</v>
+      </c>
+      <c r="E87" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="F87" s="38"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
+      <c r="L87" s="38"/>
+      <c r="N87" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="O87" s="26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B88" s="20">
+        <v>179</v>
+      </c>
+      <c r="C88" t="s">
+        <v>242</v>
+      </c>
+      <c r="E88" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="F88" s="38"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38"/>
+      <c r="L88" s="38"/>
+      <c r="N88" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="O88" s="26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B89" s="20">
+        <v>179</v>
+      </c>
+      <c r="C89" t="s">
+        <v>268</v>
+      </c>
+      <c r="E89" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="F89" s="38"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="38"/>
+      <c r="K89" s="38"/>
+      <c r="L89" s="38"/>
+      <c r="N89" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="O89" s="26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B90" s="20">
+        <v>179</v>
+      </c>
+      <c r="C90" t="s">
+        <v>276</v>
+      </c>
+      <c r="E90" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
+      <c r="K90" s="38"/>
+      <c r="L90" s="38"/>
+      <c r="N90" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="O90" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B91" s="20">
+        <v>180</v>
+      </c>
+      <c r="C91" t="s">
+        <v>281</v>
+      </c>
+      <c r="E91" t="s">
+        <v>273</v>
+      </c>
+      <c r="N91" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="O91" s="26" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="E66:L66"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+  <mergeCells count="52">
+    <mergeCell ref="E89:L89"/>
+    <mergeCell ref="E82:L82"/>
+    <mergeCell ref="E76:L76"/>
+    <mergeCell ref="E78:L78"/>
+    <mergeCell ref="E84:L84"/>
+    <mergeCell ref="E80:L80"/>
+    <mergeCell ref="E81:L81"/>
+    <mergeCell ref="E79:L79"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="E74:L74"/>
+    <mergeCell ref="E75:L75"/>
+    <mergeCell ref="E77:L77"/>
+    <mergeCell ref="E71:L71"/>
+    <mergeCell ref="E64:L64"/>
+    <mergeCell ref="E65:L65"/>
+    <mergeCell ref="E72:L72"/>
+    <mergeCell ref="E73:L73"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="I14:M14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="A11:B11"/>
@@ -2731,6 +2954,16 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E87:L87"/>
+    <mergeCell ref="E88:L88"/>
+    <mergeCell ref="E90:L90"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="E68:L68"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="I11:M11"/>
     <mergeCell ref="I5:M5"/>
@@ -2738,33 +2971,10 @@
     <mergeCell ref="I6:M6"/>
     <mergeCell ref="I7:M7"/>
     <mergeCell ref="I9:M9"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="E72:L72"/>
-    <mergeCell ref="E73:L73"/>
-    <mergeCell ref="E75:L75"/>
-    <mergeCell ref="E84:L84"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="E86:L86"/>
+    <mergeCell ref="E85:L85"/>
     <mergeCell ref="E83:L83"/>
-    <mergeCell ref="E81:L81"/>
-    <mergeCell ref="E80:L80"/>
-    <mergeCell ref="E74:L74"/>
-    <mergeCell ref="E76:L76"/>
-    <mergeCell ref="E82:L82"/>
-    <mergeCell ref="E78:L78"/>
-    <mergeCell ref="E79:L79"/>
-    <mergeCell ref="E77:L77"/>
-    <mergeCell ref="E69:L69"/>
-    <mergeCell ref="E62:L62"/>
-    <mergeCell ref="E63:L63"/>
-    <mergeCell ref="E70:L70"/>
-    <mergeCell ref="E71:L71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2779,283 +2989,283 @@
       <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="36.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
+    <col min="13" max="13" width="36.08984375" customWidth="1"/>
+    <col min="14" max="14" width="15.7265625" customWidth="1"/>
+    <col min="15" max="15" width="13.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43" t="s">
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
-      <c r="G4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="45"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="42"/>
+      <c r="I5" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="41"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="43"/>
       <c r="C6" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="I6" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="I6" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="42"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G7" s="36"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="47"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="49"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="G8" s="52"/>
-      <c r="I8" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="45"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="42"/>
+      <c r="F8" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="47"/>
+      <c r="I8" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="43"/>
       <c r="C9" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="51" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9" s="52"/>
-      <c r="I9" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="45"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="B10" s="42"/>
+      <c r="F9" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="47"/>
+      <c r="I9" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="43"/>
       <c r="C10" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="50"/>
-      <c r="I10" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="45"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="F10" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="I10" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="14" t="s">
-        <v>147</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" s="50"/>
-      <c r="I11" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="42"/>
+      <c r="F11" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="I11" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="43"/>
       <c r="C12" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="42"/>
+        <v>143</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="41"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="43"/>
       <c r="C13" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="I13" s="43" t="s">
-        <v>231</v>
-      </c>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="45"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="42"/>
+        <v>143</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="43"/>
       <c r="C14" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>230</v>
-      </c>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="45"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="42"/>
+        <v>213</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="41"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="43"/>
       <c r="C15" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I15" s="43" t="s">
-        <v>230</v>
-      </c>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="37"/>
       <c r="B16" s="37"/>
       <c r="F16" s="37"/>
@@ -3065,7 +3275,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="18" spans="3:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>0</v>
       </c>
@@ -3074,7 +3284,7 @@
       </c>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>2</v>
       </c>
@@ -3082,7 +3292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>3</v>
       </c>
@@ -3093,10 +3303,10 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>7</v>
       </c>
@@ -3110,7 +3320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H22" t="s">
         <v>11</v>
       </c>
@@ -3118,7 +3328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H23" t="s">
         <v>13</v>
       </c>
@@ -3126,7 +3336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
         <v>15</v>
       </c>
@@ -3137,7 +3347,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H25" t="s">
         <v>18</v>
       </c>
@@ -3145,7 +3355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H26" t="s">
         <v>20</v>
       </c>
@@ -3153,7 +3363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H27" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H28" t="s">
         <v>24</v>
       </c>
@@ -3169,7 +3379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H29" t="s">
         <v>26</v>
       </c>
@@ -3177,7 +3387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H30" t="s">
         <v>28</v>
       </c>
@@ -3185,50 +3395,50 @@
         <v>29</v>
       </c>
       <c r="K30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
       <c r="H31" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
         <v>167</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
-        <v>169</v>
-      </c>
-      <c r="I32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="H33" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="H34" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I34" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="H35" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I35" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>30</v>
       </c>
@@ -3239,7 +3449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>33</v>
       </c>
@@ -3250,7 +3460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B41" s="20">
         <v>0</v>
       </c>
@@ -3270,7 +3480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B42" s="20"/>
       <c r="G42">
         <v>1</v>
@@ -3285,7 +3495,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="25">
         <v>2</v>
       </c>
@@ -3301,17 +3511,17 @@
       <c r="K43" s="10">
         <v>1</v>
       </c>
-      <c r="L43" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="M43" s="41"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L43" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="M43" s="50"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="20">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G44">
         <v>3</v>
@@ -3323,10 +3533,10 @@
         <v>2</v>
       </c>
       <c r="L44" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B45" s="20">
         <v>4</v>
       </c>
@@ -3343,15 +3553,15 @@
         <v>3</v>
       </c>
       <c r="L45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B46" s="20">
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -3366,12 +3576,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B47" s="20">
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G47">
         <v>6</v>
@@ -3383,12 +3593,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B48" s="20">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G48">
         <v>7</v>
@@ -3400,10 +3610,10 @@
         <v>6</v>
       </c>
       <c r="L48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B49" s="20">
         <v>8</v>
       </c>
@@ -3417,7 +3627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B50" s="20">
         <v>9</v>
       </c>
@@ -3437,7 +3647,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B51" s="8"/>
       <c r="K51">
         <v>9</v>
@@ -3446,25 +3656,25 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B52" s="8"/>
       <c r="K52" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L52" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M52" s="19"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B53" s="8"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B58" s="20" t="s">
         <v>51</v>
       </c>
@@ -3472,16 +3682,16 @@
         <v>52</v>
       </c>
       <c r="N58" t="s">
+        <v>123</v>
+      </c>
+      <c r="O58" t="s">
         <v>124</v>
       </c>
-      <c r="O58" t="s">
+      <c r="P58" t="s">
         <v>125</v>
       </c>
-      <c r="P58" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B59" s="20">
         <v>125</v>
       </c>
@@ -3492,7 +3702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B60" s="20">
         <v>129</v>
       </c>
@@ -3503,7 +3713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B61" s="20">
         <v>105</v>
       </c>
@@ -3521,7 +3731,7 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B62" s="20">
         <v>105</v>
       </c>
@@ -3539,7 +3749,7 @@
       <c r="L62" s="38"/>
       <c r="M62" s="38"/>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B63" s="20">
         <v>105</v>
       </c>
@@ -3550,7 +3760,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B64" s="20">
         <v>105</v>
       </c>
@@ -3564,7 +3774,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B65" s="20">
         <v>105</v>
       </c>
@@ -3575,7 +3785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B66" s="20">
         <v>105</v>
       </c>
@@ -3586,7 +3796,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B67" s="20">
         <v>126</v>
       </c>
@@ -3600,7 +3810,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B68" s="20">
         <v>119</v>
       </c>
@@ -3611,7 +3821,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B69" s="20">
         <v>110</v>
       </c>
@@ -3625,7 +3835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B70" s="20">
         <v>110</v>
       </c>
@@ -3636,7 +3846,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B71" s="20">
         <v>110</v>
       </c>
@@ -3647,10 +3857,10 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B72" s="20"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B73" s="20">
         <v>121</v>
       </c>
@@ -3661,7 +3871,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B74" s="20">
         <v>126</v>
       </c>
@@ -3672,7 +3882,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B75" s="20">
         <v>126</v>
       </c>
@@ -3683,7 +3893,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B76" s="20">
         <v>131</v>
       </c>
@@ -3694,11 +3904,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:13" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="25"/>
       <c r="M77" s="24"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B78" s="20">
         <v>137</v>
       </c>
@@ -3709,7 +3919,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B79" s="20">
         <v>137</v>
       </c>
@@ -3720,10 +3930,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B80" s="20"/>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B81" s="20">
         <v>132</v>
       </c>
@@ -3734,7 +3944,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B82" s="20">
         <v>133</v>
       </c>
@@ -3745,7 +3955,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B83" s="20">
         <v>154</v>
       </c>
@@ -3756,7 +3966,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B84" s="20">
         <v>155</v>
       </c>
@@ -3767,7 +3977,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B85" s="20"/>
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
@@ -3776,12 +3986,12 @@
       <c r="I85" s="38"/>
       <c r="J85" s="38"/>
       <c r="K85" s="38"/>
-      <c r="L85" s="39"/>
+      <c r="L85" s="52"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B86" s="20"/>
       <c r="E86" s="38"/>
       <c r="F86" s="38"/>
@@ -3794,7 +4004,7 @@
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B87" s="20">
         <v>164</v>
       </c>
@@ -3805,7 +4015,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B88" s="20"/>
       <c r="C88" t="s">
         <v>106</v>
@@ -3814,26 +4024,26 @@
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B89" s="20"/>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B90" s="20"/>
     </row>
-    <row r="91" spans="2:15" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="25"/>
       <c r="C91" s="30"/>
       <c r="D91" s="30"/>
-      <c r="E91" s="48"/>
-      <c r="F91" s="48"/>
-      <c r="G91" s="48"/>
-      <c r="H91" s="48"/>
-      <c r="I91" s="48"/>
-      <c r="J91" s="48"/>
-      <c r="K91" s="48"/>
-      <c r="L91" s="48"/>
-    </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E91" s="42"/>
+      <c r="F91" s="42"/>
+      <c r="G91" s="42"/>
+      <c r="H91" s="42"/>
+      <c r="I91" s="42"/>
+      <c r="J91" s="42"/>
+      <c r="K91" s="42"/>
+      <c r="L91" s="42"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B92" s="20">
         <v>170</v>
       </c>
@@ -3844,7 +4054,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B93" s="20">
         <v>171</v>
       </c>
@@ -3855,7 +4065,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B94" s="20">
         <v>173</v>
       </c>
@@ -3869,12 +4079,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B95" s="20">
         <v>189</v>
       </c>
       <c r="E95" s="53" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F95" s="53"/>
       <c r="G95" s="53"/>
@@ -3884,15 +4094,15 @@
       <c r="K95" s="53"/>
       <c r="L95" s="53"/>
     </row>
-    <row r="96" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B96" s="20">
         <v>190</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E96" s="53" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F96" s="53"/>
       <c r="G96" s="53"/>
@@ -3902,23 +4112,46 @@
       <c r="K96" s="53"/>
       <c r="L96" s="53"/>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B97" s="20">
         <v>194</v>
       </c>
-      <c r="E97" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="F97" s="40"/>
-      <c r="G97" s="40"/>
-      <c r="H97" s="40"/>
-      <c r="I97" s="40"/>
-      <c r="J97" s="40"/>
-      <c r="K97" s="40"/>
-      <c r="L97" s="40"/>
+      <c r="E97" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="F97" s="51"/>
+      <c r="G97" s="51"/>
+      <c r="H97" s="51"/>
+      <c r="I97" s="51"/>
+      <c r="J97" s="51"/>
+      <c r="K97" s="51"/>
+      <c r="L97" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="E97:L97"/>
+    <mergeCell ref="E95:L95"/>
+    <mergeCell ref="E96:L96"/>
+    <mergeCell ref="E86:L86"/>
+    <mergeCell ref="E91:L91"/>
+    <mergeCell ref="E85:L85"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="I13:M13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="I61:M61"/>
+    <mergeCell ref="I62:M62"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:M11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="I9:M9"/>
@@ -3933,29 +4166,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="I8:M8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="E85:L85"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="I12:M12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="I61:M61"/>
-    <mergeCell ref="I62:M62"/>
-    <mergeCell ref="E97:L97"/>
-    <mergeCell ref="E95:L95"/>
-    <mergeCell ref="E96:L96"/>
-    <mergeCell ref="E86:L86"/>
-    <mergeCell ref="E91:L91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3964,157 +4174,185 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:G14"/>
+  <dimension ref="D5:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="47.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D5" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="G5" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F5" s="12" t="s">
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="E6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="F8" s="17">
         <v>42137</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D11" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F11" s="18">
         <v>42236</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D12" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F12" s="34">
         <v>42265</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D13" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F13" s="21">
         <v>42290</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="D14" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F14" s="32">
         <v>42293</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="D15" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" s="32">
+        <v>42314</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D16" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" s="32">
+        <v>42325</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>